<commit_message>
last minute typo + style
git-svn-id: https://svnserv.csiro.au/svn/ext/GeoSciML@5198 910a3654-de2c-0410-bd95-d62e98ccebcd
</commit_message>
<xml_diff>
--- a/trunk/Documents/OGC Specification/lite_to_gsml_mapping_OLR.xlsx
+++ b/trunk/Documents/OGC Specification/lite_to_gsml_mapping_OLR.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="158">
   <si>
     <t>GeologicUnitView</t>
   </si>
@@ -249,15 +249,6 @@
     <t>metadata</t>
   </si>
   <si>
-    <t>Borehole/relatedSamplingFeature/SamplingFeatureComplex/relatedSamplingFeature/Borehole/gml:identifier</t>
-  </si>
-  <si>
-    <t>Borehole/metadataProperty/href</t>
-  </si>
-  <si>
-    <t>Borehole/shape</t>
-  </si>
-  <si>
     <t>base Type gsml:MappedFeature</t>
   </si>
   <si>
@@ -273,211 +264,25 @@
     <t>specification/GeologicUnit/composition[1]/CompositionPart/material/RockMaterial/lithology</t>
   </si>
   <si>
-    <t>specification/GeologicUnit/metaDataProperty/Metadata/title (check)</t>
-  </si>
-  <si>
-    <t>specification/GeologicUnit/metaDataProperty</t>
-  </si>
-  <si>
-    <t>indexData/BoreholeDetails/purpose</t>
-  </si>
-  <si>
-    <t>downholeDrillingDetails/DrillingDetails/drillingMethod</t>
-  </si>
-  <si>
-    <t>referenceLocation/OriginPosition/elevation/coordinate</t>
-  </si>
-  <si>
-    <t>referenceLocation/OriginPosition/elevation/srsName</t>
-  </si>
-  <si>
-    <t>indexData/BoreholeDetails/operator/CI_Responsibility/party/CI_Party/name</t>
-  </si>
-  <si>
-    <t>indexData/BoreholeDetails/driller/CI_Responsibility/party/CI_Party/name</t>
-  </si>
-  <si>
-    <t>indexData/BoreholeDetails/dateOfDrilling/TM_Period/begin/TM_Instant/position</t>
-  </si>
-  <si>
-    <t>indexData/BoreholeDetails/dateOfDrilling/TM_Period/end/TM_Instant/position</t>
-  </si>
-  <si>
-    <t>indexData/BoreholeDetails/startPoint</t>
-  </si>
-  <si>
-    <t>indexData/BoreholeDetails/inclinationType</t>
-  </si>
-  <si>
-    <t>indexData/BoreholeDetails/boreholeMaterialCustodian/CI_Responsibility/party/CI_Party/name</t>
-  </si>
-  <si>
-    <t>indexData/BoreholeDetails/boreholeLength/Quantity/value</t>
-  </si>
-  <si>
-    <t>specification/Contact/identifier</t>
-  </si>
-  <si>
-    <t>specification/Contact/name[1]</t>
-  </si>
-  <si>
-    <t>specification/Contact/description</t>
-  </si>
-  <si>
-    <t>specification/Contact/contactType/(label)</t>
-  </si>
-  <si>
-    <t>specification/Contact/contactType/(uri)</t>
-  </si>
-  <si>
-    <t>specification/(uri)</t>
-  </si>
-  <si>
-    <t>specification/Contact/metaDataProperty(uri)</t>
-  </si>
-  <si>
     <t>base class : SF_Specimen</t>
   </si>
   <si>
-    <t>samplingTime/TM_Instant/position</t>
-  </si>
-  <si>
-    <t>samplingMethod/Process/description</t>
-  </si>
-  <si>
-    <t>currentLocation/EX_GeographicDescription/geographicIdentifier/MD_Identifier/code</t>
-  </si>
-  <si>
-    <t>specimentType/(uri)</t>
-  </si>
-  <si>
-    <t>specimenType/(label)</t>
-  </si>
-  <si>
-    <t>materialClass/(uri)</t>
-  </si>
-  <si>
-    <t>metadataProperty/(uri)</t>
-  </si>
-  <si>
     <t>samplingLocation</t>
   </si>
   <si>
-    <t>specification/NaturalGeomorphologicFeature/activity/(label)</t>
-  </si>
-  <si>
-    <t>specification/NaturalGeomorphologicFeature/description</t>
-  </si>
-  <si>
-    <t>specification/NaturalGeomorphologicFeature/name</t>
-  </si>
-  <si>
-    <t>specification/GeomorphologicUnit/unitDescription[1]/GeologicUnit/composition[1]/CompositionPart/material/RockMaterial/lithology</t>
-  </si>
-  <si>
-    <t>specification/{NaturalGeomorphologicFeature/naturalGeomorphologicFeatureType | AnthropogenicGeomorphologicUnit/anthropogenicGeomorphologicFeatureType}/label</t>
-  </si>
-  <si>
-    <t>specification/GeomorphologicUnit/unitDescription[1]/GeologicUnit/geologicHistory[1]/GeologicEvent/description</t>
-  </si>
-  <si>
-    <t>specification/GeomorphologicUnit/observationMethod/Category/value</t>
-  </si>
-  <si>
-    <t>specification/NaturalGeomorphologicFeature/activity/(uri)</t>
-  </si>
-  <si>
-    <t>specification(uri)</t>
-  </si>
-  <si>
     <t>base class MappedFeature</t>
   </si>
   <si>
-    <t>specification/ShearDisplacementStructure/name[1]</t>
-  </si>
-  <si>
-    <t>specification/ShearDisplacementStructure/description</t>
-  </si>
-  <si>
-    <t>specification/ShearDisplacementStructure/faultType(label)</t>
-  </si>
-  <si>
-    <t>specification/ShearDisplacementStructure/stStructureDescription/DisplacementValue/movementType(label)</t>
-  </si>
-  <si>
-    <t>specification/ShearDisplacementStructure/stStructureDescription/ShearDisplacementStructureDescription/deformationStyle(label)</t>
-  </si>
-  <si>
-    <t>specification/ShearDisplacementStructure/stStructureDescription/DisplacementValue/*</t>
-  </si>
-  <si>
-    <t>specification/ShearDisplacementStructure/geologicHistory[1]/GeologicEvent/description</t>
-  </si>
-  <si>
-    <t>specification/ShearDisplacementStructure/geologicHistory/GeologicEvent/description (merge)</t>
-  </si>
-  <si>
-    <t>observationMethod/Category/value</t>
-  </si>
-  <si>
-    <t>positionalAccuracy/Quantity/value</t>
-  </si>
-  <si>
-    <t>specification/ShearDisplacementStructure/faultType(uri)</t>
-  </si>
-  <si>
-    <t>specification/ShearDisplacementStructure/stStructureDescription/DisplacementValue/movementType(uri)</t>
-  </si>
-  <si>
-    <t>specification/ShearDisplacementStructure/stStructureDescription/ShearDisplacementStructureDescription/deformationStyle(uri)</t>
-  </si>
-  <si>
-    <t>specification/ShearDisplacementStructure/geologicHistory[$n]/GeologicEvent/youngerNamedAge</t>
-  </si>
-  <si>
-    <t>specification/ShearDisplacementStructure/geologicHistory[$n]/GeologicEvent/olderNamedAge</t>
-  </si>
-  <si>
-    <t>min(specification/ShearDisplacementStructure/geologicHistory[1]/GeologicEvent/NumericAge/yougerBoundAge/Quantity/value)</t>
-  </si>
-  <si>
-    <t>metadataProperty(uri)</t>
-  </si>
-  <si>
     <t>Base Class Observation</t>
   </si>
   <si>
     <t>problem for mapping because there is not path from obs -&gt; SamplingFeature</t>
   </si>
   <si>
-    <t>featureOfInterest/*/name</t>
-  </si>
-  <si>
-    <t>observedProperty(label)</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
-    <t>value/(uom)</t>
-  </si>
-  <si>
-    <t>procedure/(label)</t>
-  </si>
-  <si>
-    <t>featureOfInterest/(uri)</t>
-  </si>
-  <si>
-    <t>observedProperty(uri)</t>
-  </si>
-  <si>
-    <t>featureOfInterest/*/(geometry)</t>
-  </si>
-  <si>
     <t>Base Type - gsml:MappedFeature</t>
-  </si>
-  <si>
-    <t>metaDataProperty/GenericMetaData/LI_Source/description</t>
   </si>
   <si>
     <t>metaDataProperty/GenericMetaData/LI_Source/sourceCitation/identifier (uri)</t>
@@ -537,6 +342,177 @@
   </si>
   <si>
     <t>* specification/GeologicUnit/composition[1]/CompositionPart/material/RockMaterial/lithology</t>
+  </si>
+  <si>
+    <t>indexData:BoreholeDetails::purpose</t>
+  </si>
+  <si>
+    <t>downholeDrillingDetails:DrillingDetails::drillingMethod</t>
+  </si>
+  <si>
+    <t>indexData:BoreholeDetails::startPoint</t>
+  </si>
+  <si>
+    <t>indexData:BoreholeDetails::inclinationType</t>
+  </si>
+  <si>
+    <t>indexData:BoreholeDetails::driller:CI_Responsibility::party:CI_Party::name</t>
+  </si>
+  <si>
+    <t>indexData:BoreholeDetails::operator:CI_Responsibility::party:CI_Party::name</t>
+  </si>
+  <si>
+    <t>indexData:BoreholeDetails::dateOfDrilling:TM_Period::begin:TM_Instant::position</t>
+  </si>
+  <si>
+    <t>indexData:BoreholeDetails::dateOfDrilling:TM_Period::end:TM_Instant::position</t>
+  </si>
+  <si>
+    <t>indexData:BoreholeDetails::boreholeMaterialCustodian:CI_Responsibility::party:CI_Party::name</t>
+  </si>
+  <si>
+    <t>indexData:BoreholeDetails::boreholeLength:Quantity::value</t>
+  </si>
+  <si>
+    <t>referenceLocation:OriginPosition::elevationDirectPosition:::coordinate</t>
+  </si>
+  <si>
+    <t>referenceLocation:OriginPosition::elevation:srsName</t>
+  </si>
+  <si>
+    <t>metaDataProperty:MD_Metadata</t>
+  </si>
+  <si>
+    <t>relatedSamplingFeature:SamplingFeatureComplex::relatedSamplingFeature:Borehole::identifier</t>
+  </si>
+  <si>
+    <t>specification:Contact::identifier</t>
+  </si>
+  <si>
+    <t>specification:Contact::name</t>
+  </si>
+  <si>
+    <t>specification:Contact::description</t>
+  </si>
+  <si>
+    <t>specification:Contact::contactType</t>
+  </si>
+  <si>
+    <t>specification::Contact:contactType</t>
+  </si>
+  <si>
+    <t>specification</t>
+  </si>
+  <si>
+    <t>specification::Contact::metaDataProperty</t>
+  </si>
+  <si>
+    <t>samplingTime:TM_Instant::position</t>
+  </si>
+  <si>
+    <t>currentLocation:EX_GeographicDescription::geographicIdentifier:MD_Identifier::code</t>
+  </si>
+  <si>
+    <t>specification:GeologicUnit::metaDataProperty:(…):CI_Citation</t>
+  </si>
+  <si>
+    <t>metaDataProperty:(…):CI_Citation</t>
+  </si>
+  <si>
+    <t>metaDataProperty(…):CI_Citation</t>
+  </si>
+  <si>
+    <t>metadataProperty:(…):DQ_PositionalAccuracy</t>
+  </si>
+  <si>
+    <t>specimentType</t>
+  </si>
+  <si>
+    <t>metadataProperty</t>
+  </si>
+  <si>
+    <t>specification:NaturalGeomorphologicFeature::name</t>
+  </si>
+  <si>
+    <t>specification:NaturalGeomorphologicFeature::description</t>
+  </si>
+  <si>
+    <t>specification:NaturalGeomorphologicFeature:activity</t>
+  </si>
+  <si>
+    <t>specification:NaturalGeomorphologicFeature::naturalGeomorphologicFeatureType |specification:AnthropogenicGeomorphologicUnit::anthropogenicGeomorphologicFeatureType</t>
+  </si>
+  <si>
+    <t>specification:GeomorphologicUnit::unitDescription:GeologicUnit::composition:CompositionPart::material:RockMaterial::lithology</t>
+  </si>
+  <si>
+    <t>specification:GeomorphologicUnit::unitDescription:GeologicUnit::geologicHistory:GeologicEvent::description</t>
+  </si>
+  <si>
+    <t>specification:GeomorphologicUnit::observationMethod:Category::value</t>
+  </si>
+  <si>
+    <t>positionalAccuracy::value</t>
+  </si>
+  <si>
+    <t>specification:NaturalGeomorphologicFeature::activity</t>
+  </si>
+  <si>
+    <t>specification:GeologicUnit:metaDataProperty</t>
+  </si>
+  <si>
+    <t>specification:ShearDisplacementStructure::name</t>
+  </si>
+  <si>
+    <t>specification:ShearDisplacementStructure::description</t>
+  </si>
+  <si>
+    <t>specification:ShearDisplacementStructure::faultType</t>
+  </si>
+  <si>
+    <t>specification:ShearDisplacementStructure::stStructureDescription:DisplacementValue::movementType</t>
+  </si>
+  <si>
+    <t>specification:ShearDisplacementStructure::stStructureDescription:ShearDisplacementStructureDescription::deformationStyle</t>
+  </si>
+  <si>
+    <t>specification:ShearDisplacementStructure::stStructureDescription:DisplacementValue</t>
+  </si>
+  <si>
+    <t>specification:ShearDisplacementStructure::geologicHistory:GeologicEvent::description</t>
+  </si>
+  <si>
+    <t>observationMethod:Category::value</t>
+  </si>
+  <si>
+    <t>positionalAccuracy:Quantity::value</t>
+  </si>
+  <si>
+    <t>specification:ShearDisplacementStructure::geologicHistory:GeologicEvent:youngerNamedAge</t>
+  </si>
+  <si>
+    <t>specification:ShearDisplacementStructure::geologicHistory:GeologicEvent::olderNamedAge</t>
+  </si>
+  <si>
+    <t>specification:ShearDisplacementStructure::geologicHistory:GeologicEvent::numericAge:NumericAgeRange::youngerBoundAge:Quantity::value</t>
+  </si>
+  <si>
+    <t>specification:ShearDisplacementStructure::geologicHistory:GeologicEvent::numericAge:NumericAgeRange::olderBoundAge:Quantity::value</t>
+  </si>
+  <si>
+    <t>specification:ShearDisplacementStructure::geologicHistory:GeologicEvent</t>
+  </si>
+  <si>
+    <t>featureOfInterest:(…)::name</t>
+  </si>
+  <si>
+    <t>procedure</t>
+  </si>
+  <si>
+    <t>metaDataProperty</t>
+  </si>
+  <si>
+    <t>featureOfInterest:(…):GM_Object</t>
   </si>
 </sst>
 </file>
@@ -634,7 +610,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -922,14 +898,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C160"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C135" sqref="C135"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="118.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.140625" style="3" customWidth="1"/>
     <col min="3" max="3" width="70.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -938,12 +914,12 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>152</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
-        <v>164</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -959,7 +935,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>156</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -967,7 +943,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -975,7 +951,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -983,7 +959,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -991,7 +967,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>165</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -999,7 +975,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>161</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1007,7 +983,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>162</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -1015,7 +991,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>163</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1023,7 +999,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>157</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1039,7 +1015,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>153</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1047,7 +1023,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1055,7 +1031,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1063,7 +1039,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>160</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1071,7 +1047,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>158</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1079,7 +1055,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>159</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1087,7 +1063,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>155</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1095,7 +1071,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>154</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1151,7 +1127,7 @@
         <v>24</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1164,7 +1140,7 @@
         <v>26</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1172,7 +1148,7 @@
         <v>27</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1180,7 +1156,7 @@
         <v>28</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1188,7 +1164,7 @@
         <v>29</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1196,7 +1172,7 @@
         <v>30</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1204,7 +1180,7 @@
         <v>31</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1212,7 +1188,7 @@
         <v>32</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1220,7 +1196,7 @@
         <v>33</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1228,7 +1204,7 @@
         <v>34</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1236,7 +1212,7 @@
         <v>35</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1244,7 +1220,7 @@
         <v>36</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1260,15 +1236,15 @@
         <v>12</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>37</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>77</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1276,7 +1252,7 @@
         <v>19</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1289,7 +1265,7 @@
         <v>21</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>79</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1302,7 +1278,7 @@
         <v>38</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>152</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1310,7 +1286,7 @@
         <v>1</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1318,7 +1294,7 @@
         <v>2</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1326,7 +1302,7 @@
         <v>3</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1334,7 +1310,7 @@
         <v>39</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1358,7 +1334,7 @@
         <v>12</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -1366,7 +1342,7 @@
         <v>40</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1374,7 +1350,7 @@
         <v>18</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1382,7 +1358,7 @@
         <v>19</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1408,7 +1384,7 @@
         <v>41</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1440,7 +1416,7 @@
         <v>43</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>111</v>
+        <v>43</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -1455,13 +1431,16 @@
       <c r="A76" t="s">
         <v>11</v>
       </c>
+      <c r="B76" s="5" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>45</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -1469,7 +1448,7 @@
         <v>46</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>108</v>
+        <v>46</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1477,7 +1456,7 @@
         <v>47</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -1485,7 +1464,7 @@
         <v>12</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1493,7 +1472,7 @@
         <v>48</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1501,7 +1480,7 @@
         <v>49</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>112</v>
+        <v>44</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -1509,7 +1488,7 @@
         <v>19</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -1522,7 +1501,7 @@
         <v>21</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -1535,7 +1514,7 @@
         <v>50</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>124</v>
+        <v>84</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -1551,7 +1530,7 @@
         <v>2</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -1559,7 +1538,7 @@
         <v>3</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -1567,7 +1546,7 @@
         <v>51</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1575,23 +1554,23 @@
         <v>52</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>6</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>7</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -1599,7 +1578,7 @@
         <v>10</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -1607,7 +1586,7 @@
         <v>11</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>11</v>
+        <v>137</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -1615,7 +1594,7 @@
         <v>12</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -1623,7 +1602,7 @@
         <v>53</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -1641,12 +1620,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>14</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -1664,7 +1643,7 @@
         <v>18</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -1672,7 +1651,7 @@
         <v>19</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>86</v>
+        <v>139</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -1698,7 +1677,7 @@
         <v>58</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -1714,7 +1693,7 @@
         <v>2</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -1722,7 +1701,7 @@
         <v>3</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -1730,23 +1709,23 @@
         <v>59</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>60</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>61</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -1754,7 +1733,7 @@
         <v>62</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -1762,7 +1741,7 @@
         <v>7</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -1770,7 +1749,7 @@
         <v>10</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -1778,7 +1757,7 @@
         <v>11</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -1786,7 +1765,7 @@
         <v>12</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -1794,7 +1773,7 @@
         <v>63</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -1802,28 +1781,31 @@
         <v>64</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>65</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>15</v>
       </c>
+      <c r="B129" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>16</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -1831,15 +1813,15 @@
         <v>17</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>8</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1847,7 +1829,7 @@
         <v>9</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -1855,7 +1837,7 @@
         <v>18</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -1863,7 +1845,7 @@
         <v>19</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -1889,7 +1871,7 @@
         <v>66</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>142</v>
+        <v>85</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -1908,7 +1890,7 @@
         <v>2</v>
       </c>
       <c r="C143" t="s">
-        <v>143</v>
+        <v>86</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -1940,7 +1922,7 @@
         <v>69</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
@@ -1948,7 +1930,7 @@
         <v>70</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -1956,7 +1938,7 @@
         <v>71</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>146</v>
+        <v>87</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
@@ -1964,7 +1946,7 @@
         <v>72</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>147</v>
+        <v>87</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
@@ -1972,20 +1954,23 @@
         <v>10</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>11</v>
       </c>
+      <c r="B152" s="5" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>12</v>
       </c>
       <c r="B153" s="5" t="s">
-        <v>85</v>
+        <v>125</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -1993,7 +1978,7 @@
         <v>73</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>149</v>
+        <v>69</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -2001,7 +1986,7 @@
         <v>74</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>150</v>
+        <v>70</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
@@ -2009,7 +1994,7 @@
         <v>19</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>86</v>
+        <v>156</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
@@ -2027,7 +2012,7 @@
         <v>21</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -2047,7 +2032,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2059,7 +2044,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>